<commit_message>
changes in chrome driver and data sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/Datasheets/Invalid_CreditCard_Num.xlsx
+++ b/src/main/resources/Datasheets/Invalid_CreditCard_Num.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F633B5A-CAA8-4905-8756-AD46DE313F59}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD01AB1-7122-4D28-953C-88C6406E89FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,9 +37,6 @@
     <t>ExpiryDate</t>
   </si>
   <si>
-    <t>03/20</t>
-  </si>
-  <si>
     <t>4811 1111 1111 1114</t>
   </si>
   <si>
@@ -47,6 +44,9 @@
   </si>
   <si>
     <t>4811 1111 1111 1113</t>
+  </si>
+  <si>
+    <t>09/20</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -461,18 +461,18 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="D2" s="3">
         <v>123</v>

</xml_diff>